<commit_message>
read sub menu item from excel
</commit_message>
<xml_diff>
--- a/map1.xlsx
+++ b/map1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xzjzb\PycharmProjects\CG\tool\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xzjzb\Desktop\DirectX\MapEditor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2516EF81-3C94-4789-B469-799BBBCDACC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EF1A281-0160-4D17-8416-9F4C32F1120D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3680" windowWidth="16200" windowHeight="10060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20085" yWindow="4965" windowWidth="28800" windowHeight="15345" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Map" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>オブジェクトNAME</t>
   </si>
@@ -39,20 +39,31 @@
     <t>道</t>
   </si>
   <si>
-    <t>blue</t>
-  </si>
-  <si>
     <t>MapSizeX</t>
   </si>
   <si>
     <t>MapSizeY</t>
+  </si>
+  <si>
+    <t>建物１</t>
+    <rPh sb="0" eb="2">
+      <t>タテモノ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Purple</t>
+  </si>
+  <si>
+    <t>LightPink</t>
+    <phoneticPr fontId="1"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -95,7 +106,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="標準" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -397,13 +408,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2:F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1">
         <v>0</v>
       </c>
@@ -423,7 +434,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>0</v>
       </c>
@@ -437,7 +448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>0</v>
       </c>
@@ -451,7 +462,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>0</v>
       </c>
@@ -465,7 +476,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6">
       <c r="A5">
         <v>0</v>
       </c>
@@ -479,7 +490,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6">
       <c r="A6">
         <v>0</v>
       </c>
@@ -502,18 +513,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="4" width="20.6328125" customWidth="1"/>
+    <col min="1" max="4" width="20.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -527,15 +538,26 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C2">
         <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -549,23 +571,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B1">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2">
         <v>6</v>

</xml_diff>

<commit_message>
add sub menu item save
</commit_message>
<xml_diff>
--- a/map1.xlsx
+++ b/map1.xlsx
@@ -1,87 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xzjzb\Desktop\DirectX\MapEditor\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EF1A281-0160-4D17-8416-9F4C32F1120D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20085" yWindow="4965" windowWidth="28800" windowHeight="15345" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="1185" yWindow="4365" windowWidth="28800" windowHeight="15345" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Map" sheetId="1" r:id="rId1"/>
-    <sheet name="Submenu" sheetId="2" r:id="rId2"/>
-    <sheet name="MapInfo" sheetId="3" r:id="rId3"/>
+    <sheet name="Map" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Submenu" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="MapInfo" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
-  <si>
-    <t>オブジェクトNAME</t>
-  </si>
-  <si>
-    <t>コマの色</t>
-  </si>
-  <si>
-    <t>フラグ</t>
-  </si>
-  <si>
-    <t>オブジェクトアドレス</t>
-  </si>
-  <si>
-    <t>道</t>
-  </si>
-  <si>
-    <t>MapSizeX</t>
-  </si>
-  <si>
-    <t>MapSizeY</t>
-  </si>
-  <si>
-    <t>建物１</t>
-    <rPh sb="0" eb="2">
-      <t>タテモノ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Purple</t>
-  </si>
-  <si>
-    <t>LightPink</t>
-    <phoneticPr fontId="1"/>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="ＭＳ Ｐゴシック"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <name val="ＭＳ Ｐゴシック"/>
+      <charset val="128"/>
+      <family val="3"/>
       <sz val="6"/>
-      <name val="ＭＳ Ｐゴシック"/>
-      <family val="3"/>
-      <charset val="128"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -100,24 +55,83 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -405,196 +419,240 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2:F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="13.5"/>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1">
-        <v>0</v>
-      </c>
-      <c r="B1">
-        <v>0</v>
-      </c>
-      <c r="C1">
-        <v>0</v>
-      </c>
-      <c r="D1">
+    <row r="1">
+      <c r="A1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1" t="n">
         <v>1</v>
       </c>
-      <c r="E1">
-        <v>0</v>
-      </c>
-      <c r="F1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3">
-        <v>0</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
+      <c r="E1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>0</v>
+      </c>
+      <c r="B3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
-      <c r="A4">
-        <v>0</v>
-      </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
+    <row r="4">
+      <c r="A4" t="n">
+        <v>0</v>
+      </c>
+      <c r="B4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
-      <c r="A5">
-        <v>0</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6">
-        <v>0</v>
-      </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
+    <row r="5">
+      <c r="A5" t="n">
+        <v>0</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>0</v>
+      </c>
+      <c r="B6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" t="n">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="4" width="20.625" customWidth="1"/>
+    <col width="20.625" customWidth="1" min="1" max="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>オブジェクトNAME</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>コマの色</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>フラグ</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>オブジェクトアドレス</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>道</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>LightPink</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>建物１</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Purple</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>建物</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Aqua</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="13.5"/>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1">
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>MapSizeX</t>
+        </is>
+      </c>
+      <c r="B1" t="n">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>MapSizeY</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
         <v>6</v>
       </c>
-      <c r="B2">
-        <v>6</v>
-      </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
sub menu item temp save
</commit_message>
<xml_diff>
--- a/map1.xlsx
+++ b/map1.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="1185" yWindow="4365" windowWidth="28800" windowHeight="15345" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="7650" yWindow="5535" windowWidth="28800" windowHeight="15345" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Map" sheetId="1" state="visible" r:id="rId1"/>
@@ -534,10 +534,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+      <selection activeCell="A8" sqref="A8:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="13.5"/>
@@ -610,6 +610,141 @@
       </c>
       <c r="C4" t="n">
         <v>4</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>建物3</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Orange</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>建物5</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Tomato</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>建物6</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Yellow</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>建物222</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Green</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>建物42412</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>IndianRed</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>建物3434</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>LightBlue</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>建物31231</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Navy</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>建物231</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Cyan</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>建物434</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Salmon</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
write obj file address to excel file
</commit_message>
<xml_diff>
--- a/map1.xlsx
+++ b/map1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="7650" yWindow="5535" windowWidth="28800" windowHeight="15345" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Map" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Submenu" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="MapInfo" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Map" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Submenu" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="MapInfo" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -534,7 +534,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A8" sqref="A8:XFD12"/>
@@ -745,6 +745,66 @@
       </c>
       <c r="C13" t="n">
         <v>14</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>house</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>SkyBlue</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>15</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>C:/Users/xzjzb/PycharmProjects/MapEditor/data/model/house/house.obj</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>house2</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Maroon</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>11</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>/data/model/house/house.obj</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>建物house</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Tan</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>16</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>data/model/house/house.obj</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
complete move & add & remove
</commit_message>
<xml_diff>
--- a/map1.xlsx
+++ b/map1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="7650" yWindow="5535" windowWidth="28800" windowHeight="15345" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="16335" yWindow="3855" windowWidth="28800" windowHeight="15345" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Map" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Submenu" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="MapInfo" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Map" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Submenu" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="MapInfo" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -424,26 +424,26 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:F6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="13.5"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B1" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C1" t="n">
         <v>0</v>
       </c>
       <c r="D1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E1" t="n">
         <v>0</v>
@@ -454,15 +454,21 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
       </c>
       <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -474,10 +480,16 @@
         <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D3" t="n">
-        <v>1</v>
+        <v>10</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -488,10 +500,16 @@
         <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>10</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -502,10 +520,16 @@
         <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="D5" t="n">
-        <v>3</v>
+        <v>19</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -516,10 +540,70 @@
         <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="D6" t="n">
-        <v>3</v>
+        <v>19</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>0</v>
+      </c>
+      <c r="B7" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>0</v>
+      </c>
+      <c r="B8" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="n">
+        <v>8</v>
+      </c>
+      <c r="C9" t="n">
+        <v>1</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -536,8 +620,8 @@
   </sheetPr>
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="13.5"/>
@@ -834,7 +918,7 @@
         </is>
       </c>
       <c r="B1" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2">
@@ -844,7 +928,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>